<commit_message>
exam_manage added and connected
</commit_message>
<xml_diff>
--- a/test_system/static/patches/Students.xlsx
+++ b/test_system/static/patches/Students.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/grishaoganov/Downloads/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2E9FBCC-CBE7-2449-8AE0-E30E067BDCD0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="94">
   <si>
     <t>Студенческий билет</t>
   </si>
@@ -106,13 +112,205 @@
   </si>
   <si>
     <t>adserebrennikov@edu.hse.ru</t>
+  </si>
+  <si>
+    <t>gsoganov@edu.hse.ru</t>
+  </si>
+  <si>
+    <t>Оганов</t>
+  </si>
+  <si>
+    <t>Григорий</t>
+  </si>
+  <si>
+    <t>М181БПИНЖ234</t>
+  </si>
+  <si>
+    <t>М181БПИНЖ235</t>
+  </si>
+  <si>
+    <t>Клюкин</t>
+  </si>
+  <si>
+    <t>Валерий</t>
+  </si>
+  <si>
+    <t>kdklukin@edu.hse.ru</t>
+  </si>
+  <si>
+    <t>Дубина</t>
+  </si>
+  <si>
+    <t>Дмитрий</t>
+  </si>
+  <si>
+    <t>Олегович</t>
+  </si>
+  <si>
+    <t>dodubina@edu.hse.ru</t>
+  </si>
+  <si>
+    <t>М181БПИНЖ236</t>
+  </si>
+  <si>
+    <t>М181БПИНЖ237</t>
+  </si>
+  <si>
+    <t>Торилов</t>
+  </si>
+  <si>
+    <t>Михайлович</t>
+  </si>
+  <si>
+    <t>dmtorilov@edu.hse.ru</t>
+  </si>
+  <si>
+    <t>Емельяненко</t>
+  </si>
+  <si>
+    <t>Викторович</t>
+  </si>
+  <si>
+    <t>dvemelyanenko@edu.hse.ru</t>
+  </si>
+  <si>
+    <t>Редникина</t>
+  </si>
+  <si>
+    <t>Дарья</t>
+  </si>
+  <si>
+    <t>Юрьевна</t>
+  </si>
+  <si>
+    <t>durednikina@edu.hse.ru</t>
+  </si>
+  <si>
+    <t>Загитов</t>
+  </si>
+  <si>
+    <t>Асгар</t>
+  </si>
+  <si>
+    <t>Ильшатович</t>
+  </si>
+  <si>
+    <t>aizagitov@edu.hse.ru</t>
+  </si>
+  <si>
+    <t>М181БПИНЖ238</t>
+  </si>
+  <si>
+    <t>М181БПИНЖ239</t>
+  </si>
+  <si>
+    <t>М181БПИНЖ240</t>
+  </si>
+  <si>
+    <t>М181БПИНЖ241</t>
+  </si>
+  <si>
+    <t>Белавенцев</t>
+  </si>
+  <si>
+    <t>Евгеньевич</t>
+  </si>
+  <si>
+    <t>vebelavencev@edu.hse.ru</t>
+  </si>
+  <si>
+    <t>Оралин</t>
+  </si>
+  <si>
+    <t>М181БПИНЖ242</t>
+  </si>
+  <si>
+    <t>М181БПИНЖ243</t>
+  </si>
+  <si>
+    <t>Илларион</t>
+  </si>
+  <si>
+    <t>Владимирович</t>
+  </si>
+  <si>
+    <t>ivoralin@edu.hse.ru</t>
+  </si>
+  <si>
+    <t>Соколов</t>
+  </si>
+  <si>
+    <t>Семен</t>
+  </si>
+  <si>
+    <t>Константинович</t>
+  </si>
+  <si>
+    <t>sksokolov@edu.hse.ru</t>
+  </si>
+  <si>
+    <t>М181БПИНЖ244</t>
+  </si>
+  <si>
+    <t>М181БПИНЖ245</t>
+  </si>
+  <si>
+    <t>М181БПИНЖ246</t>
+  </si>
+  <si>
+    <t>М181БПИНЖ247</t>
+  </si>
+  <si>
+    <t>Сафина</t>
+  </si>
+  <si>
+    <t>Алия</t>
+  </si>
+  <si>
+    <t>Наилевна</t>
+  </si>
+  <si>
+    <t>ansafina@edu.hse.ru</t>
+  </si>
+  <si>
+    <t>Карпин</t>
+  </si>
+  <si>
+    <t>Николаевич</t>
+  </si>
+  <si>
+    <t>ankarpin@edu.hse.ru</t>
+  </si>
+  <si>
+    <t>Измайлов</t>
+  </si>
+  <si>
+    <t>Александрович</t>
+  </si>
+  <si>
+    <t>aaizmailov@edu.hse.ru</t>
+  </si>
+  <si>
+    <t>Силина</t>
+  </si>
+  <si>
+    <t>Полина</t>
+  </si>
+  <si>
+    <t>Викторовна</t>
+  </si>
+  <si>
+    <t>pvsilina@edu.hse.ru</t>
+  </si>
+  <si>
+    <t>Прикладная математика и информатика</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,6 +323,15 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -193,14 +400,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -208,11 +413,16 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -220,6 +430,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -268,7 +481,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -301,9 +514,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -336,6 +566,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -511,148 +758,470 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
-      <c r="G1" s="4"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="G1" s="3"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="2" t="s">
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="3" t="s">
+      <c r="E3" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="3" t="s">
+      <c r="E4" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" s="3" t="s">
+      <c r="E5" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="3" t="s">
+      <c r="E6" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -662,29 +1231,45 @@
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="G7" r:id="rId1" xr:uid="{1046DC76-B3A9-6646-ACA6-F462BB0878D4}"/>
+    <hyperlink ref="G8" r:id="rId2" xr:uid="{76EBAFE9-0ADB-6942-A1BB-8A7249FA2A34}"/>
+    <hyperlink ref="G9" r:id="rId3" xr:uid="{FD694EB4-129D-0F45-85FA-B582BA4F69A7}"/>
+    <hyperlink ref="G10" r:id="rId4" xr:uid="{F672F595-8D3B-6B45-B54B-8AF1E7653DAA}"/>
+    <hyperlink ref="G11" r:id="rId5" xr:uid="{ACA5F03C-D0F2-FC49-B0C4-DD3709A798AF}"/>
+    <hyperlink ref="G12" r:id="rId6" xr:uid="{F5148760-44E8-0846-9562-A0EC2671FDA0}"/>
+    <hyperlink ref="G13" r:id="rId7" xr:uid="{8E49FC2A-DD39-B243-9E64-D7D88255B153}"/>
+    <hyperlink ref="G14" r:id="rId8" xr:uid="{07121177-1217-824D-A5D2-E8CB1CFF2C23}"/>
+    <hyperlink ref="G15" r:id="rId9" xr:uid="{A23EDA26-1DA1-6F47-A593-83AFBE42F05B}"/>
+    <hyperlink ref="G16" r:id="rId10" xr:uid="{FB380D84-46C5-3D46-ABAE-333DB1EDA88F}"/>
+    <hyperlink ref="G17" r:id="rId11" xr:uid="{BF223DF9-2499-AC4C-AEAF-33F408491F5F}"/>
+    <hyperlink ref="G18" r:id="rId12" xr:uid="{95BB1256-9B4E-BA42-B402-97213255A383}"/>
+    <hyperlink ref="G19" r:id="rId13" xr:uid="{CB20D558-3C28-EF44-9FFA-EF3DFFCED1A6}"/>
+    <hyperlink ref="G20" r:id="rId14" xr:uid="{369E1EC6-BFFD-3640-AAE9-D4CF42346B84}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>